<commit_message>
fix: added emp id in sheet to manage the data
</commit_message>
<xml_diff>
--- a/public/sample-files/sample_hours.xlsx
+++ b/public/sample-files/sample_hours.xlsx
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">EmpId</t>
+  </si>
   <si>
     <t xml:space="preserve">Employee</t>
   </si>
   <si>
     <t xml:space="preserve">Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate</t>
   </si>
   <si>
     <t xml:space="preserve">Alice</t>
@@ -128,13 +134,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -158,56 +172,90 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.43"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>170</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="D2" s="3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>150</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>170</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <v>165</v>
       </c>
+      <c r="D5" s="3" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="2"/>
+      <c r="D12" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>